<commit_message>
Final Update User Story 2
</commit_message>
<xml_diff>
--- a/scrum/Defesa Sprint 2 - 2023.xlsx
+++ b/scrum/Defesa Sprint 2 - 2023.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{B314CFC2-C346-4E49-AC59-9519C98B3EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D2FC42-A5CA-4F34-9FC1-1C95BF246C9E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A260DC98-20A0-40CD-97CC-E3E08DC420AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENTREGA PRODUTO" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Produto Final Operacional</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>PROJETO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipe </t>
   </si>
   <si>
     <r>
@@ -217,9 +214,6 @@
 Equipe</t>
   </si>
   <si>
-    <t>Estudante 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Valor 
 Máximo </t>
   </si>
@@ -242,24 +236,12 @@
   </si>
   <si>
     <t>Feedback</t>
-  </si>
-  <si>
-    <t>Estudante 2</t>
-  </si>
-  <si>
-    <t>Estudante 3</t>
   </si>
   <si>
     <t>NOTA =</t>
   </si>
   <si>
     <t>NOTA AJUSTADA =</t>
-  </si>
-  <si>
-    <t>Estudante 4</t>
-  </si>
-  <si>
-    <t>Estudante 5</t>
   </si>
   <si>
     <r>
@@ -348,15 +330,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> (texto padrão ARO)
+      <t>: Realizar Login de Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -374,15 +356,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Persona
+      <t>: Idealizador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -400,15 +382,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">PBI
+      <t>: Realizar Login de Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -426,15 +408,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> Benefício / Resultado da Feature do PBI
+      <t>: Ter Acesso as Funções de Idealizador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -479,15 +461,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">cenário 1
+      <t>: Preciso acessar meu perfil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -505,15 +487,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">ação do usuário esperada
+      <t>: Preencho meus dados corretamente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -531,15 +513,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">resultado esperado, com mensagem ao usuário
+      <t>: Conecto na minha conta e posso visualizar meu perfil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -575,15 +557,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">cenário 2
+      <t>: Preciso acessar meu perfil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -601,15 +583,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">ação do usuário (não adequada ou que pode gerar erro)
+      <t>: Preencho minha senha incorretamente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -627,16 +609,1216 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> resultado trata o problema, com mensagem ao usuário</t>
-    </r>
+      <t>: Não consigo realizar o login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PBI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Realizar Cadastro de Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>COMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Colaborador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>POSSO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Realizar Cadastro do Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PARA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Conseguir um Trabalho</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:	
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Preciso achar emprego na minha área</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Realizo o cadastro de usuário e preencho um email que ainda não foi utilizado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Consigo criar uma conta e aplicar para um emprego em projetos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Preciso achar emprego na minha área</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Realizo o cadastro de usuário e preencho um email que já foi utilizado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Não consigo criar uma conta e aplicar para emprego em projetos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PBI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Filtrar Áreas de Interesse do Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>COMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Colaborador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>POSSO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Filtrar Áreas de Interesse do Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PARA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">: Conseguir um trabalho
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:	
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Preciso achar um emprego na minha área</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Escolho a minha área de interesse e existem projetos cadastrados nela</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: É mostrado para mim uma lista dos projetos da área</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Preciso achar um emprego na minha área</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Escolho a minha área de interesse e não existem projetos cadastrados nela</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: É mostrado para mim uma mensagem informando que não existem projetos da área</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PBI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Gerenciar Cadastro de Ideias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>COMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Idealizador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>POSSO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Gerenciar Cadastro de Ideias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PARA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Definir Cargos Necessários Para a Realização do Projeto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:	
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Preciso de uma equipe de colaboradores para realizar um projeto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Gerencio o cadastro de ideias e preencho o formulário corretamente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Posso criar uma postagem com minha ideia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Preciso de uma equipe de colaboradores para realizar um projeto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Gerencio o cadastro de ideias e preencho o nome da ideia com menos de dois caracteres</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Não consigo criar uma postagem com minha ideia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PBI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Realizar Doações para um Projeto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>COMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Doador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>POSSO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Realizar Doações para um Projeto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PARA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Auxiliar na Concretização do Projeto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:	
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Achei um projeto do meu interesse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Insiro os dados para a doação com valores inteiros e positivos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Consigo realizar a doação e ajudar o projeto a se concretizar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>CRITÉRIO DE ACEITE 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DADO QUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Achei um projeto do meu interesse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>QUANDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Insiro os dados para a doação com valores não inteiros e negativos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ENTÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Não consigo realizar a doação e é mostrado para mim uma mensagem informando que não foi possível realizar a doação</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Equipe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Got an Idea</t>
+    </r>
+  </si>
+  <si>
+    <t>Estudante 1: Diogo Bonet</t>
+  </si>
+  <si>
+    <t>Estudante 2: Felipe Vermelho</t>
+  </si>
+  <si>
+    <t>Estudante 3: Gabriel Mocellin</t>
+  </si>
+  <si>
+    <t>Estudante 4: João Trigo</t>
+  </si>
+  <si>
+    <t>Estudante 5: João Pedro Mendes</t>
+  </si>
+  <si>
+    <t>Estudante 6: Nicolas Peralta</t>
   </si>
 </sst>
 </file>
@@ -646,7 +1828,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1448,7 +2630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1553,93 +2735,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1703,15 +2924,6 @@
     <xf numFmtId="9" fontId="14" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1748,36 +2960,9 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1786,6 +2971,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF3ACDEA"/>
       <color rgb="FF008000"/>
       <color rgb="FFF2D10E"/>
       <color rgb="FF006600"/>
@@ -2071,11 +3257,11 @@
   </sheetPr>
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16:Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -2097,165 +3283,165 @@
     <col min="25" max="25" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30" customHeight="1" thickBot="1">
-      <c r="I1" s="50" t="s">
+    <row r="1" spans="1:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="50" t="s">
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="53"/>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:25" ht="54.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:25" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="55" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="55" t="s">
+      <c r="N2" s="57"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="59" t="s">
+      <c r="Q2" s="61"/>
+      <c r="R2" s="62"/>
+      <c r="T2" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="61"/>
-      <c r="T2" s="62" t="s">
+      <c r="U2" s="75"/>
+      <c r="V2" s="76"/>
+    </row>
+    <row r="3" spans="1:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="63"/>
-      <c r="V2" s="64"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="79"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="87"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="91" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" ht="21.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="69" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="U3" s="74"/>
-      <c r="V3" s="75"/>
-      <c r="W3" s="78" t="s">
+    <row r="4" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="42.75" customHeight="1">
-      <c r="A4" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88"/>
+      <c r="B4" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="65"/>
       <c r="H4" s="5"/>
       <c r="I4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="77"/>
+      <c r="L4" s="90"/>
       <c r="M4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="P4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="S4" s="73"/>
+      <c r="S4" s="86"/>
       <c r="T4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="V4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="W4" s="79"/>
+      <c r="W4" s="92"/>
     </row>
-    <row r="5" spans="1:25" s="4" customFormat="1" ht="120" customHeight="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88"/>
+    <row r="5" spans="1:25" s="4" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16">
         <v>6</v>
       </c>
       <c r="J5" s="17"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="85"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="98"/>
       <c r="M5" s="16">
         <v>2</v>
       </c>
@@ -2280,63 +3466,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A6" s="49"/>
-      <c r="B6" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="88"/>
+    <row r="6" spans="1:25" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="B6" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="65"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="80">
+      <c r="I6" s="93">
         <f>(I5*J5)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="81"/>
+      <c r="J6" s="94"/>
       <c r="K6" s="28"/>
-      <c r="M6" s="80">
+      <c r="M6" s="93">
         <f>(M5*N5)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="81"/>
-      <c r="P6" s="80">
+      <c r="N6" s="94"/>
+      <c r="P6" s="93">
         <f>(P5*Q5)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="81"/>
+      <c r="Q6" s="94"/>
       <c r="R6" s="25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="S6" s="22">
         <f>S5</f>
         <v>0</v>
       </c>
-      <c r="T6" s="82">
+      <c r="T6" s="95">
         <f>(T5*U5)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="83"/>
+      <c r="U6" s="96"/>
       <c r="V6" s="26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="W6" s="27">
         <f>S6*T6/10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="26.25" customHeight="1">
-      <c r="A7" s="49"/>
-      <c r="B7" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="88"/>
+    <row r="7" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="5"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -2352,16 +3538,16 @@
       <c r="U7"/>
       <c r="V7"/>
     </row>
-    <row r="8" spans="1:25" ht="26.25" customHeight="1">
-      <c r="A8" s="49"/>
-      <c r="B8" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="88"/>
+    <row r="8" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
+      <c r="B8" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="5"/>
       <c r="I8"/>
       <c r="J8"/>
@@ -2377,116 +3563,118 @@
       <c r="U8"/>
       <c r="V8"/>
     </row>
-    <row r="9" spans="1:25" ht="48.75" customHeight="1">
+    <row r="9" spans="1:25" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="B9" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="5"/>
-      <c r="P9" s="101" t="s">
+      <c r="P9" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
+      <c r="U9" s="67"/>
+      <c r="V9" s="67"/>
+      <c r="W9" s="67"/>
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68"/>
+    </row>
+    <row r="10" spans="1:25" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="P10" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="102"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="102"/>
-      <c r="T9" s="102"/>
-      <c r="U9" s="102"/>
-      <c r="V9" s="102"/>
-      <c r="W9" s="102"/>
-      <c r="X9" s="102"/>
-      <c r="Y9" s="103"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="73"/>
+      <c r="W10" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="X10" s="73"/>
+      <c r="Y10" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" ht="48.75" customHeight="1">
-      <c r="A10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="P10" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="105"/>
-      <c r="R10" s="106" t="s">
-        <v>31</v>
-      </c>
-      <c r="S10" s="107"/>
-      <c r="T10" s="108"/>
-      <c r="U10" s="106" t="s">
-        <v>32</v>
-      </c>
-      <c r="V10" s="108"/>
-      <c r="W10" s="106" t="s">
-        <v>33</v>
-      </c>
-      <c r="X10" s="108"/>
-      <c r="Y10" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="219.75" customHeight="1">
+    <row r="11" spans="1:25" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="109" t="s">
-        <v>35</v>
+      <c r="B11" s="36" t="s">
+        <v>32</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="29">
         <v>1</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
-      <c r="P11" s="89" t="str">
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="46"/>
+      <c r="P11" s="99" t="str">
         <f>B4</f>
-        <v>Estudante 1</v>
-      </c>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="94"/>
-      <c r="S11" s="95"/>
-      <c r="T11" s="96"/>
-      <c r="U11" s="97"/>
-      <c r="V11" s="98"/>
-      <c r="W11" s="99"/>
-      <c r="X11" s="100"/>
+        <v>Estudante 1: Diogo Bonet</v>
+      </c>
+      <c r="Q11" s="100"/>
+      <c r="R11" s="104"/>
+      <c r="S11" s="105"/>
+      <c r="T11" s="106"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="110"/>
       <c r="Y11" s="12">
         <f>$W$6 * W11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="204" customHeight="1">
+    <row r="12" spans="1:25" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="109" t="s">
-        <v>35</v>
+      <c r="B12" s="36" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
@@ -2499,32 +3687,32 @@
       <c r="K12" s="30">
         <v>1</v>
       </c>
-      <c r="L12" s="43"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
-      <c r="P12" s="89" t="str">
+      <c r="L12" s="44"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="46"/>
+      <c r="P12" s="99" t="str">
         <f>B5</f>
-        <v>Estudante 2</v>
-      </c>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="94"/>
-      <c r="S12" s="95"/>
-      <c r="T12" s="96"/>
-      <c r="U12" s="97"/>
-      <c r="V12" s="98"/>
-      <c r="W12" s="99"/>
-      <c r="X12" s="100"/>
+        <v>Estudante 2: Felipe Vermelho</v>
+      </c>
+      <c r="Q12" s="100"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="105"/>
+      <c r="T12" s="106"/>
+      <c r="U12" s="107"/>
+      <c r="V12" s="108"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="110"/>
       <c r="Y12" s="12">
         <f>$W$6 * W12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="204" customHeight="1">
+    <row r="13" spans="1:25" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
-      <c r="B13" s="109" t="s">
-        <v>35</v>
+      <c r="B13" s="36" t="s">
+        <v>30</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
@@ -2537,32 +3725,32 @@
       <c r="K13" s="30">
         <v>2</v>
       </c>
-      <c r="L13" s="43"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="P13" s="89" t="str">
+      <c r="L13" s="44"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="46"/>
+      <c r="P13" s="99" t="str">
         <f>B6</f>
-        <v>Estudante 3</v>
-      </c>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="95"/>
-      <c r="T13" s="96"/>
-      <c r="U13" s="97"/>
-      <c r="V13" s="98"/>
-      <c r="W13" s="99"/>
-      <c r="X13" s="100"/>
+        <v>Estudante 3: Gabriel Mocellin</v>
+      </c>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="105"/>
+      <c r="T13" s="106"/>
+      <c r="U13" s="107"/>
+      <c r="V13" s="108"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="110"/>
       <c r="Y13" s="12">
         <f>$W$6 * W13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="204" customHeight="1">
+    <row r="14" spans="1:25" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
-      <c r="B14" s="109" t="s">
-        <v>35</v>
+      <c r="B14" s="36" t="s">
+        <v>31</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
@@ -2575,32 +3763,32 @@
       <c r="K14" s="30">
         <v>2</v>
       </c>
-      <c r="L14" s="43"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="45"/>
-      <c r="P14" s="89" t="str">
+      <c r="L14" s="44"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="46"/>
+      <c r="P14" s="99" t="str">
         <f>B7</f>
-        <v>Estudante 4</v>
-      </c>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="94"/>
-      <c r="S14" s="95"/>
-      <c r="T14" s="96"/>
-      <c r="U14" s="97"/>
-      <c r="V14" s="98"/>
-      <c r="W14" s="99"/>
-      <c r="X14" s="100"/>
+        <v>Estudante 4: João Trigo</v>
+      </c>
+      <c r="Q14" s="100"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="105"/>
+      <c r="T14" s="106"/>
+      <c r="U14" s="107"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="109"/>
+      <c r="X14" s="110"/>
       <c r="Y14" s="12">
         <f>$W$6 * W14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="204" customHeight="1">
+    <row r="15" spans="1:25" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5</v>
       </c>
-      <c r="B15" s="109" t="s">
-        <v>35</v>
+      <c r="B15" s="36" t="s">
+        <v>33</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -2613,27 +3801,27 @@
       <c r="K15" s="30">
         <v>2</v>
       </c>
-      <c r="L15" s="43"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="45"/>
-      <c r="P15" s="89" t="str">
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="46"/>
+      <c r="P15" s="99" t="str">
         <f>B8</f>
-        <v>Estudante 5</v>
-      </c>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="91"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="91"/>
-      <c r="U15" s="92"/>
-      <c r="V15" s="92"/>
-      <c r="W15" s="93"/>
-      <c r="X15" s="93"/>
+        <v>Estudante 5: João Pedro Mendes</v>
+      </c>
+      <c r="Q15" s="100"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="101"/>
+      <c r="U15" s="102"/>
+      <c r="V15" s="102"/>
+      <c r="W15" s="103"/>
+      <c r="X15" s="103"/>
       <c r="Y15" s="12">
         <f>$W$6 * W15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="44.25" customHeight="1">
+    <row r="16" spans="1:25" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6</v>
       </c>
@@ -2647,11 +3835,27 @@
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="45"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="46"/>
+      <c r="P16" s="99" t="str">
+        <f>B9</f>
+        <v>Estudante 6: Nicolas Peralta</v>
+      </c>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="101"/>
+      <c r="S16" s="101"/>
+      <c r="T16" s="101"/>
+      <c r="U16" s="102"/>
+      <c r="V16" s="102"/>
+      <c r="W16" s="103"/>
+      <c r="X16" s="103"/>
+      <c r="Y16" s="12">
+        <f>$W$6 * W16</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" ht="38.25" customHeight="1">
+    <row r="17" spans="1:22" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -2665,9 +3869,9 @@
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
       <c r="O17" s="31"/>
       <c r="P17" s="31"/>
       <c r="Q17" s="31"/>
@@ -2677,7 +3881,7 @@
       <c r="U17"/>
       <c r="V17"/>
     </row>
-    <row r="18" spans="1:22" ht="32.25" customHeight="1">
+    <row r="18" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -2691,14 +3895,14 @@
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="10"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:22" ht="32.25" customHeight="1">
+    <row r="19" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -2712,14 +3916,14 @@
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:22" ht="32.25" customHeight="1">
+    <row r="20" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10</v>
       </c>
@@ -2733,11 +3937,11 @@
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
     </row>
-    <row r="21" spans="1:22" ht="32.25" customHeight="1">
+    <row r="21" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>11</v>
       </c>
@@ -2751,11 +3955,11 @@
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
     </row>
-    <row r="22" spans="1:22" ht="32.25" customHeight="1">
+    <row r="22" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12</v>
       </c>
@@ -2769,14 +3973,18 @@
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
     </row>
-    <row r="23" spans="1:22" ht="35.1" customHeight="1"/>
-    <row r="24" spans="1:22" ht="46.5" customHeight="1"/>
+    <row r="23" spans="1:22" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:22" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="94">
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="W16:X16"/>
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="R12:T12"/>
     <mergeCell ref="U12:V12"/>

</xml_diff>